<commit_message>
Adding stuff in test plan
- ADC
- DAC
- Speedcheck
</commit_message>
<xml_diff>
--- a/2020-2021/PCB/Test_Plan_PCB.xlsx
+++ b/2020-2021/PCB/Test_Plan_PCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11800025\Documents\GitHub\intelliflow\2020-2021\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2988C26A-5AD3-4BF2-A707-6DBF519D57A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA71FC39-120A-40C5-8D64-BC86CC3730D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C0FA133-E7D3-49B5-A26D-63F79587637D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="87">
   <si>
     <t>Testplan PCB</t>
   </si>
@@ -169,9 +169,6 @@
     <t>GPIO8 (DRYD ADC)</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recieving data on </t>
   </si>
   <si>
@@ -263,12 +260,6 @@
   </si>
   <si>
     <t>SPI DAC 70504</t>
-  </si>
-  <si>
-    <t>Measerment SCLK  ADC 1247</t>
-  </si>
-  <si>
-    <t>Measerment  SCLK DAC 70504</t>
   </si>
   <si>
     <t>Recieved Data on</t>
@@ -302,6 +293,21 @@
       </rPr>
       <t xml:space="preserve"> test should fail</t>
     </r>
+  </si>
+  <si>
+    <t>Connection possible with SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output current is </t>
+  </si>
+  <si>
+    <t>Measerment SCLK  to ADC 1247</t>
+  </si>
+  <si>
+    <t>Measerment  SCLK to DAC 70504</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> min is 480 ns or around 2 Mhz , should fail</t>
   </si>
 </sst>
 </file>
@@ -345,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,12 +379,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,7 +479,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -794,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435DD37B-4652-4CB1-BE49-B8C09510E9E7}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="64" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1006,7 +1005,7 @@
     <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
@@ -1050,7 +1049,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="6"/>
       <c r="E28" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1063,7 +1062,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1076,7 +1075,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1089,19 +1088,18 @@
         <v>5</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
@@ -1154,19 +1152,19 @@
         <v>8</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -1266,7 +1264,7 @@
         <v>8</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -1344,66 +1342,73 @@
     <row r="62" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="11" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="B63" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A65" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="14"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
+      <c r="B65" s="14"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A66" s="12" t="s">
+    <row r="66" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A67" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B67" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D67" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="9"/>
     </row>
     <row r="68" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="B68" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9"/>
     </row>
     <row r="69" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="2"/>
+      <c r="B69" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9"/>
+    </row>
+    <row r="70" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="14"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1413,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40509FE-E360-49B3-BC2C-20962025613A}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView zoomScale="58" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,6 +1430,7 @@
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -1432,19 +1438,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="7"/>
@@ -1452,7 +1458,7 @@
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="7"/>
@@ -1460,7 +1466,7 @@
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="7"/>
@@ -1468,7 +1474,7 @@
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="7"/>
@@ -1476,7 +1482,7 @@
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="7"/>
@@ -1484,7 +1490,7 @@
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="7"/>
@@ -1492,7 +1498,7 @@
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="7"/>
@@ -1500,7 +1506,7 @@
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="7"/>
@@ -1526,22 +1532,22 @@
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
@@ -1549,7 +1555,7 @@
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="7"/>
@@ -1563,19 +1569,19 @@
     <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="7"/>
@@ -1583,7 +1589,7 @@
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="7"/>
@@ -1599,7 +1605,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -1607,43 +1613,43 @@
     </row>
     <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
@@ -1651,133 +1657,139 @@
     <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C29" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="14"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B41" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="7"/>
-    </row>
-    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C43" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B45" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B47" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="7"/>
+      <c r="E47" s="23" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
@@ -1787,43 +1799,43 @@
     </row>
     <row r="51" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C51" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B54" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B55" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="7"/>
@@ -1831,40 +1843,40 @@
     <row r="57" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C57" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B59" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B60" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B61" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="7"/>

</xml_diff>

<commit_message>
Testing completed PCB v1
- Commenting/finalizing testplan PCB
- Update psoc codes
</commit_message>
<xml_diff>
--- a/2020-2021/PCB/Test_Plan_PCB.xlsx
+++ b/2020-2021/PCB/Test_Plan_PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11800025\Documents\GitHub\intelliflow\2020-2021\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D562CE0E-3D74-4A7B-8F10-CCA3BF7094DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09EAF87-6481-44FD-8953-B3E380CBD6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C0FA133-E7D3-49B5-A26D-63F79587637D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C0FA133-E7D3-49B5-A26D-63F79587637D}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB v1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="115">
   <si>
     <t>Testplan PCB</t>
   </si>
@@ -322,9 +322,6 @@
     <t>optional</t>
   </si>
   <si>
-    <t>08/11/2020 =  Test completed  no errors</t>
-  </si>
-  <si>
     <t>https://learn.sparkfun.com/tutorials/serial-communication/all</t>
   </si>
   <si>
@@ -364,12 +361,6 @@
     <t>Recieved data</t>
   </si>
   <si>
-    <t>No data on PSOC4</t>
-  </si>
-  <si>
-    <t>Garbage on ESP32 and no data on PSOC4</t>
-  </si>
-  <si>
     <t>1,5 MHZ</t>
   </si>
   <si>
@@ -377,21 +368,6 @@
   </si>
   <si>
     <t>SPI full duplex on (sending and recieving data psoc 4)</t>
-  </si>
-  <si>
-    <r>
-      <t>22/11/2020 = test completed ,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> only 12MHZ on MISO ?</t>
-    </r>
   </si>
   <si>
     <r>
@@ -407,6 +383,39 @@
       </rPr>
       <t xml:space="preserve"> Note: bitwise &lt;&lt; 1 is needed while sending to psoc , loss LSB bit</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Somtimes corruption in data </t>
+  </si>
+  <si>
+    <t>08/11/2020 =  Test completed with psoc4 no errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More corruption in data </t>
+  </si>
+  <si>
+    <r>
+      <t>22/11/2020 = test completed,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> only 12MHZ on MISO ?</t>
+    </r>
+  </si>
+  <si>
+    <t>27/11/2020 = Lost LSB fit is from the PSOC SPI block https://community.cypress.com/thread/26206?start=0&amp;tstart=0</t>
+  </si>
+  <si>
+    <t>27/11/2020 = changing external clock doenst have effect on SPI block psoc https://community.cypress.com/thread/26206?start=0&amp;tstart=0</t>
+  </si>
+  <si>
+    <t>cancelled due to hardware problems</t>
   </si>
 </sst>
 </file>
@@ -458,7 +467,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,6 +501,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,7 +613,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1009,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435DD37B-4652-4CB1-BE49-B8C09510E9E7}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1486,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -1563,7 +1579,7 @@
     <row r="60" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>5</v>
@@ -1581,7 +1597,7 @@
         <v>8</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -1606,26 +1622,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="14" t="s">
         <v>8</v>
       </c>
@@ -1633,13 +1655,13 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="12" t="s">
         <v>40</v>
       </c>
@@ -1653,23 +1675,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="9"/>
-    </row>
-    <row r="72" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E71" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="11" t="s">
         <v>79</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="9"/>
-    </row>
-    <row r="73" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E72" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="14" t="s">
         <v>8</v>
       </c>
@@ -1686,16 +1714,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40509FE-E360-49B3-BC2C-20962025613A}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="77" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="B20" zoomScale="60" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.85546875" customWidth="1"/>
-    <col min="2" max="2" width="120.140625" customWidth="1"/>
+    <col min="2" max="2" width="158.28515625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
     <col min="5" max="5" width="76.28515625" customWidth="1"/>
@@ -1806,23 +1834,23 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
-      <c r="B12" s="16" t="s">
-        <v>93</v>
+      <c r="B12" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
-      <c r="B13" s="27" t="s">
-        <v>92</v>
+      <c r="B13" s="28" t="s">
+        <v>91</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1854,7 +1882,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1865,7 +1893,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="7"/>
       <c r="E17" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1917,13 +1945,13 @@
         <v>8</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
-      <c r="B24" s="27" t="s">
-        <v>94</v>
+      <c r="B24" s="28" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1934,7 +1962,7 @@
         <v>69</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>55</v>
@@ -1946,19 +1974,19 @@
     <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
@@ -1967,7 +1995,7 @@
     </row>
     <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>5</v>
@@ -1976,7 +2004,7 @@
     </row>
     <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B30" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>5</v>
@@ -1985,284 +2013,343 @@
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
     </row>
     <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="14" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="D36" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
       <c r="B37" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="7"/>
+        <v>98</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>103</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="14"/>
+      <c r="B41" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+      <c r="B42" s="14"/>
+    </row>
+    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>110</v>
+      <c r="B43" s="14" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16"/>
+      <c r="B44" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B46" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-      <c r="B45" s="21" t="s">
+    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B46" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="7"/>
+      <c r="E47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="7"/>
       <c r="E48" t="s">
-        <v>6</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B49" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="7"/>
+      <c r="E49" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
       <c r="B50" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="7"/>
+      <c r="E50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D52" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="21" t="s">
+    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B52" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B53" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="7"/>
+      <c r="E53" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B54" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="7"/>
-      <c r="E54" s="23" t="s">
+      <c r="E54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B55" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="7"/>
+      <c r="E55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B56" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="23" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="14" t="s">
+    <row r="58" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="22"/>
-    </row>
-    <row r="58" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="17" t="s">
+      <c r="B58" s="22"/>
+    </row>
+    <row r="60" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B60" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D60" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="21" t="s">
+    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="7"/>
-    </row>
-    <row r="60" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B60" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="7"/>
-    </row>
-    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B61" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="7"/>
+      <c r="E61" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B62" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="7"/>
+      <c r="E62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B63" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="7"/>
+      <c r="E63" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="2"/>
       <c r="B64" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="7"/>
+      <c r="E64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C66" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D66" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="21" t="s">
+    <row r="67" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B66" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B67" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="7"/>
-    </row>
-    <row r="68" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B68" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="7"/>
-    </row>
-    <row r="70" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="E68" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B69" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="7"/>
+      <c r="E69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B70" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="7"/>
+      <c r="E70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>